<commit_message>
Implemented SSN and CC Discovery
</commit_message>
<xml_diff>
--- a/Import_Template.xlsx
+++ b/Import_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects-teamhbs\files-o365-readiness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heartlandbusinesssystems-my.sharepoint.com/personal/tnabbefeld_hbs_net/Documents/Documents/GitHub/files-o365-readiness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5E6461-8A7C-44B9-AD5C-165EEBA672F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{DF5E6461-8A7C-44B9-AD5C-165EEBA672F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2C59981-07D3-413B-A524-0B433861837E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7050" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>SourceDirectory</t>
   </si>
@@ -28,13 +28,7 @@
     <t>BatchNumber</t>
   </si>
   <si>
-    <t>C:\docs\adelev</t>
-  </si>
-  <si>
-    <t>C:\docs\meganb</t>
-  </si>
-  <si>
-    <t>C:\docs\admin</t>
+    <t>C:\Users\tnabbefeld\Documents\test</t>
   </si>
 </sst>
 </file>
@@ -875,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,28 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="\\somefileserver\share1" xr:uid="{51946B69-1A01-478D-A67F-9688418E3279}"/>
-    <hyperlink ref="A3" r:id="rId2" display="\\myfileshare\jbaldwin$\" xr:uid="{78D0A5E9-46E4-4EC2-98FC-25D591D8912D}"/>
-    <hyperlink ref="A4" r:id="rId3" display="\\myfileshare\jbaldwin$\" xr:uid="{69032546-8C01-4CFD-A1C2-A9A9E52AB0FB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>